<commit_message>
updated Cotabato City pop data
</commit_message>
<xml_diff>
--- a/data101_data/pop_per_reg.xlsx
+++ b/data101_data/pop_per_reg.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JUPYTER FILES\DATA101\Project\Final Project Dash App\D101_Interactive_Visualization_Project\data101_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3598B47F-2AC9-480B-AC64-13FB00C2A03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F8AF25-9C7A-4213-BA25-9C9904A72F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,7 +347,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +362,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -396,16 +414,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,10 +1059,10 @@
         <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
-        <v>215348</v>
+        <v>41</v>
+      </c>
+      <c r="C30" s="2">
+        <v>324539</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>